<commit_message>
added current working directory to base path functionality.
</commit_message>
<xml_diff>
--- a/publication/idpt_settings.xlsx
+++ b/publication/idpt_settings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenzie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenzie/PythonProjects/idpt/publication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D25A37-8D28-554F-A45B-FBBE37D9883E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16612CED-847F-FC4E-9ECF-FBCC68CE445D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20280" yWindow="-2420" windowWidth="19920" windowHeight="21040" xr2:uid="{AA802539-9F53-9341-8CC5-E0E4EA5358C3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>{'pad': 5}</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>results</t>
+  </si>
+  <si>
+    <t>base_dir</t>
+  </si>
+  <si>
+    <t>os.getcwd()</t>
   </si>
 </sst>
 </file>
@@ -537,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0864D04-0BF9-8648-839C-9DF9A1D0592A}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,170 +564,178 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" t="s">
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>